<commit_message>
Exe 06 - nnn
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C064DB3-C58B-2F44-8B43-02A39954C178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8858763B-91B6-E247-9A67-4B91FF0A2F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
   </bookViews>
   <sheets>
     <sheet name="If Else" sheetId="1" r:id="rId1"/>
+    <sheet name="Exe 06 - nnn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>構成</t>
   </si>
@@ -140,6 +141,84 @@
   </si>
   <si>
     <t xml:space="preserve">    print ("X = 1")</t>
+  </si>
+  <si>
+    <t>exe_06_nnn.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_06_nnn.py</t>
+  </si>
+  <si>
+    <t># Input     : Nhập vào số tự nhiên n (0 &lt; n &lt; 10)</t>
+  </si>
+  <si>
+    <t># Output    : In ra tổng của n + nn + nnn</t>
+  </si>
+  <si>
+    <t># Ví dụ     : Nhập 5, in ra tổng 5 + 55 + 555 = 615</t>
+  </si>
+  <si>
+    <t>try:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      myNumber     = int(input("Nhập vào số tự nhiên n (0 &lt; n &lt; 10): "))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      if(myNumber &gt; 0 and myNumber &lt; 10):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            n1    = int( "%s" % myNumber )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            n2    = int( "%s%s" % (myNumber, myNumber))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            n3    = int( "%s%s%s" % (myNumber, myNumber, myNumber) )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            print ("{n1} + {n2} + {n3} = {result}".format(n1 = n1, n2 = n2, n3 = n3, result = n1 + n2 + n3))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      else :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            print ("Giá trị nhập vào không hợp lệ")</t>
+  </si>
+  <si>
+    <t>except ValueError:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      print ("Giá trị nhập vào phải là số tự nhiên")</t>
+  </si>
+  <si>
+    <t>Trường hợp chưa dùng try-catch</t>
+  </si>
+  <si>
+    <t>myNumber     = int(input("Nhập vào số tự nhiên n (0 &lt; n &lt; 10): "))</t>
+  </si>
+  <si>
+    <t>if(myNumber &gt; 0 and myNumber &lt; 10):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    n1    = int( "%s" % myNumber )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    n2    = int( "%s%s" % (myNumber, myNumber))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    n3    = int( "%s%s%s" % (myNumber, myNumber, myNumber) )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print ("{n1} + {n2} + {n3} = {result}".format(n1 = n1, n2 = n2, n3 = n3, result = n1 + n2 + n3))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print ("Giá trị nhập vào không hợp lệ")</t>
+  </si>
+  <si>
+    <t>python3 exe_06_nnn.py</t>
+  </si>
+  <si>
+    <t>Có sử dụng try-catch</t>
   </si>
 </sst>
 </file>
@@ -287,10 +366,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +425,158 @@
         <a:xfrm>
           <a:off x="952499" y="9029700"/>
           <a:ext cx="11589597" cy="1168400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88899</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>74476</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2A3FF0-0B42-876C-FCAE-890ED13BDCD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914399" y="9842500"/>
+          <a:ext cx="12368077" cy="2222500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C892DE6-CCFD-CD20-672D-6CE8F7791332}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1104900" y="11772900"/>
+          <a:ext cx="330200" cy="4152900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101358</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{983B7407-9E18-811D-E3E8-D7BAF11BC664}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939800" y="17411700"/>
+          <a:ext cx="12369558" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -656,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B34BA4E-ADB9-0F46-B627-FD0732ACC69E}">
   <dimension ref="A3:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,7 +994,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
-      <c r="D17" s="11" t="s">
+      <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="5"/>
@@ -838,7 +1069,7 @@
       <c r="F26" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -853,63 +1084,54 @@
       <c r="B31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="12"/>
       <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B32" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="12"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="12"/>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="12"/>
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="12"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="12"/>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="12"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="12"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="12"/>
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -918,7 +1140,7 @@
       <c r="D40" s="10"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="12" t="s">
         <v>26</v>
       </c>
       <c r="B43" s="2"/>
@@ -939,130 +1161,33 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-      <c r="B44" s="12" t="s">
+      <c r="B44" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
       <c r="P44" s="5"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
       <c r="P46" s="5"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
       <c r="P47" s="5"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
       <c r="P48" s="5"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
       <c r="P49" s="5"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
       <c r="P50" s="5"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
@@ -1087,4 +1212,1661 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF950FC-648E-824C-9D05-ADFE4B6493D6}">
+  <dimension ref="A3:Q156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="4"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="5"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="14"/>
+      <c r="P56" s="14"/>
+      <c r="Q56" s="5"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="14"/>
+      <c r="P57" s="14"/>
+      <c r="Q57" s="5"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="14"/>
+      <c r="P58" s="14"/>
+      <c r="Q58" s="5"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="14"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="5"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="10"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="3"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="5"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="14"/>
+      <c r="Q65" s="5"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="14"/>
+      <c r="P66" s="14"/>
+      <c r="Q66" s="5"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="14"/>
+      <c r="P67" s="14"/>
+      <c r="Q67" s="5"/>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="14"/>
+      <c r="N68" s="14"/>
+      <c r="O68" s="14"/>
+      <c r="P68" s="14"/>
+      <c r="Q68" s="5"/>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="14"/>
+      <c r="Q69" s="5"/>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="14"/>
+      <c r="P70" s="14"/>
+      <c r="Q70" s="5"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
+      <c r="P71" s="14"/>
+      <c r="Q71" s="5"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="14"/>
+      <c r="Q72" s="5"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="14"/>
+      <c r="Q73" s="5"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14"/>
+      <c r="P74" s="14"/>
+      <c r="Q74" s="5"/>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+      <c r="Q75" s="5"/>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="Q76" s="5"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="5"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="14"/>
+      <c r="P78" s="14"/>
+      <c r="Q78" s="5"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
+      <c r="N79" s="14"/>
+      <c r="O79" s="14"/>
+      <c r="P79" s="14"/>
+      <c r="Q79" s="5"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="14"/>
+      <c r="P80" s="14"/>
+      <c r="Q80" s="5"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="14"/>
+      <c r="Q81" s="5"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
+      <c r="N82" s="14"/>
+      <c r="O82" s="14"/>
+      <c r="P82" s="14"/>
+      <c r="Q82" s="5"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="14"/>
+      <c r="O83" s="14"/>
+      <c r="P83" s="14"/>
+      <c r="Q83" s="5"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+      <c r="N84" s="14"/>
+      <c r="O84" s="14"/>
+      <c r="P84" s="14"/>
+      <c r="Q84" s="5"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="4"/>
+      <c r="B85" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
+      <c r="N85" s="14"/>
+      <c r="O85" s="14"/>
+      <c r="P85" s="14"/>
+      <c r="Q85" s="5"/>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" s="4"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="14"/>
+      <c r="N86" s="14"/>
+      <c r="O86" s="14"/>
+      <c r="P86" s="14"/>
+      <c r="Q86" s="5"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
+      <c r="N87" s="14"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="14"/>
+      <c r="Q87" s="5"/>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="14"/>
+      <c r="N88" s="14"/>
+      <c r="O88" s="14"/>
+      <c r="P88" s="14"/>
+      <c r="Q88" s="5"/>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="14"/>
+      <c r="Q89" s="5"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" s="4"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="14"/>
+      <c r="P90" s="14"/>
+      <c r="Q90" s="5"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" s="4"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
+      <c r="N91" s="14"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="14"/>
+      <c r="Q91" s="5"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="14"/>
+      <c r="N92" s="14"/>
+      <c r="O92" s="14"/>
+      <c r="P92" s="14"/>
+      <c r="Q92" s="5"/>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="14"/>
+      <c r="N93" s="14"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="14"/>
+      <c r="Q93" s="5"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="9"/>
+      <c r="K94" s="9"/>
+      <c r="L94" s="9"/>
+      <c r="M94" s="9"/>
+      <c r="N94" s="9"/>
+      <c r="O94" s="9"/>
+      <c r="P94" s="9"/>
+      <c r="Q94" s="10"/>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B138" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="3"/>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B139" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14"/>
+      <c r="E139" s="14"/>
+      <c r="F139" s="14"/>
+      <c r="G139" s="14"/>
+      <c r="H139" s="14"/>
+      <c r="I139" s="5"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B140" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="14"/>
+      <c r="G140" s="14"/>
+      <c r="H140" s="14"/>
+      <c r="I140" s="5"/>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B141" s="4"/>
+      <c r="C141" s="14"/>
+      <c r="D141" s="14"/>
+      <c r="E141" s="14"/>
+      <c r="F141" s="14"/>
+      <c r="G141" s="14"/>
+      <c r="H141" s="14"/>
+      <c r="I141" s="5"/>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B142" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C142" s="14"/>
+      <c r="D142" s="14"/>
+      <c r="E142" s="14"/>
+      <c r="F142" s="14"/>
+      <c r="G142" s="14"/>
+      <c r="H142" s="14"/>
+      <c r="I142" s="5"/>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B143" s="4"/>
+      <c r="C143" s="14"/>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="14"/>
+      <c r="G143" s="14"/>
+      <c r="H143" s="14"/>
+      <c r="I143" s="5"/>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B144" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C144" s="14"/>
+      <c r="D144" s="14"/>
+      <c r="E144" s="14"/>
+      <c r="F144" s="14"/>
+      <c r="G144" s="14"/>
+      <c r="H144" s="14"/>
+      <c r="I144" s="5"/>
+    </row>
+    <row r="145" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B145" s="4"/>
+      <c r="C145" s="14"/>
+      <c r="D145" s="14"/>
+      <c r="E145" s="14"/>
+      <c r="F145" s="14"/>
+      <c r="G145" s="14"/>
+      <c r="H145" s="14"/>
+      <c r="I145" s="5"/>
+    </row>
+    <row r="146" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B146" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C146" s="14"/>
+      <c r="D146" s="14"/>
+      <c r="E146" s="14"/>
+      <c r="F146" s="14"/>
+      <c r="G146" s="14"/>
+      <c r="H146" s="14"/>
+      <c r="I146" s="5"/>
+    </row>
+    <row r="147" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B147" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="14"/>
+      <c r="G147" s="14"/>
+      <c r="H147" s="14"/>
+      <c r="I147" s="5"/>
+    </row>
+    <row r="148" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B148" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C148" s="14"/>
+      <c r="D148" s="14"/>
+      <c r="E148" s="14"/>
+      <c r="F148" s="14"/>
+      <c r="G148" s="14"/>
+      <c r="H148" s="14"/>
+      <c r="I148" s="5"/>
+    </row>
+    <row r="149" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B149" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C149" s="14"/>
+      <c r="D149" s="14"/>
+      <c r="E149" s="14"/>
+      <c r="F149" s="14"/>
+      <c r="G149" s="14"/>
+      <c r="H149" s="14"/>
+      <c r="I149" s="5"/>
+    </row>
+    <row r="150" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B150" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C150" s="14"/>
+      <c r="D150" s="14"/>
+      <c r="E150" s="14"/>
+      <c r="F150" s="14"/>
+      <c r="G150" s="14"/>
+      <c r="H150" s="14"/>
+      <c r="I150" s="5"/>
+    </row>
+    <row r="151" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B151" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C151" s="14"/>
+      <c r="D151" s="14"/>
+      <c r="E151" s="14"/>
+      <c r="F151" s="14"/>
+      <c r="G151" s="14"/>
+      <c r="H151" s="14"/>
+      <c r="I151" s="5"/>
+    </row>
+    <row r="152" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B152" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C152" s="14"/>
+      <c r="D152" s="14"/>
+      <c r="E152" s="14"/>
+      <c r="F152" s="14"/>
+      <c r="G152" s="14"/>
+      <c r="H152" s="14"/>
+      <c r="I152" s="5"/>
+    </row>
+    <row r="153" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B153" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C153" s="14"/>
+      <c r="D153" s="14"/>
+      <c r="E153" s="14"/>
+      <c r="F153" s="14"/>
+      <c r="G153" s="14"/>
+      <c r="H153" s="14"/>
+      <c r="I153" s="5"/>
+    </row>
+    <row r="154" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B154" s="4"/>
+      <c r="C154" s="14"/>
+      <c r="D154" s="14"/>
+      <c r="E154" s="14"/>
+      <c r="F154" s="14"/>
+      <c r="G154" s="14"/>
+      <c r="H154" s="14"/>
+      <c r="I154" s="5"/>
+    </row>
+    <row r="155" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B155" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C155" s="14"/>
+      <c r="D155" s="14"/>
+      <c r="E155" s="14"/>
+      <c r="F155" s="14"/>
+      <c r="G155" s="14"/>
+      <c r="H155" s="14"/>
+      <c r="I155" s="5"/>
+    </row>
+    <row r="156" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B156" s="8"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 07 - range 01
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE43971-D42E-7B4E-B550-8CFB3ECB063F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D63A04-11DB-2A4A-9F1A-49444CAAA13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="4" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
+    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="5" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
   </bookViews>
   <sheets>
     <sheet name="If Else" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="For" sheetId="3" r:id="rId3"/>
     <sheet name="While" sheetId="4" r:id="rId4"/>
     <sheet name="Break Continue" sheetId="5" r:id="rId5"/>
+    <sheet name="Exe 07 - range 01" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="114">
   <si>
     <t>構成</t>
   </si>
@@ -342,6 +343,45 @@
   </si>
   <si>
     <t>Nhảy sang bước i khác</t>
+  </si>
+  <si>
+    <t>exe_07_range_01.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_07_range_01.py</t>
+  </si>
+  <si>
+    <t># Input     : [a,b] và n (ví dụ n = 3)</t>
+  </si>
+  <si>
+    <t># Output    : In ra list [a1, b1, a2, b2, a3, b3]</t>
+  </si>
+  <si>
+    <t>myList = ['x', 'y', 'z']</t>
+  </si>
+  <si>
+    <t>n = 2</t>
+  </si>
+  <si>
+    <t>result = []</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for index in range(1, n + 1):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        elm = "{}-{}".format(item, index)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        result.append(elm)</t>
+  </si>
+  <si>
+    <t>print(result)</t>
+  </si>
+  <si>
+    <t>python3 exe_07_range_01.py</t>
+  </si>
+  <si>
+    <t>index = 1, 2</t>
   </si>
 </sst>
 </file>
@@ -946,6 +986,108 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>520292</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB753CA7-9DFF-7F3B-9383-245CBFBDC3FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="927100" y="10655300"/>
+          <a:ext cx="11150192" cy="1206500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74667BE8-2011-AC19-3E08-AC8882BBF1CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="7886700"/>
+          <a:ext cx="1422400" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3180,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E74769E7-4771-D64D-82DF-B7DC58579374}">
   <dimension ref="A3:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3316,7 +3458,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
-      <c r="D21" s="13" t="s">
+      <c r="D21" t="s">
         <v>77</v>
       </c>
       <c r="F21" s="5"/>
@@ -3435,17 +3577,6 @@
         <v>88</v>
       </c>
       <c r="C35" s="3"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
       <c r="O35" s="5"/>
       <c r="P35" s="5"/>
     </row>
@@ -3455,17 +3586,6 @@
         <v>79</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
     </row>
@@ -3475,17 +3595,6 @@
         <v>80</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
     </row>
@@ -3495,17 +3604,6 @@
         <v>89</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
     </row>
@@ -3515,17 +3613,6 @@
         <v>90</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
     </row>
@@ -3535,21 +3622,12 @@
         <v>91</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="14" t="s">
+      <c r="D40" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" t="s">
         <v>99</v>
       </c>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
@@ -3559,17 +3637,6 @@
         <v>92</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
     </row>
@@ -3577,163 +3644,49 @@
       <c r="A42" s="4"/>
       <c r="B42" s="8"/>
       <c r="C42" s="10"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
       <c r="O42" s="5"/>
       <c r="P42" s="5"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
       <c r="O43" s="5"/>
       <c r="P43" s="5"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-      <c r="B44" s="14" t="s">
+      <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
       <c r="O44" s="5"/>
       <c r="P44" s="5"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
       <c r="O45" s="5"/>
       <c r="P45" s="5"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
       <c r="O46" s="5"/>
       <c r="P46" s="5"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
       <c r="O48" s="5"/>
       <c r="P48" s="5"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
       <c r="O49" s="5"/>
       <c r="P49" s="5"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
       <c r="O50" s="5"/>
       <c r="P50" s="5"/>
     </row>
@@ -3757,38 +3710,10 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
       <c r="P52" s="5"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
       <c r="P53" s="5"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
@@ -3817,17 +3742,6 @@
         <v>95</v>
       </c>
       <c r="C55" s="3"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
     </row>
@@ -3837,17 +3751,6 @@
         <v>79</v>
       </c>
       <c r="C56" s="5"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
     </row>
@@ -3857,17 +3760,6 @@
         <v>80</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
     </row>
@@ -3877,17 +3769,6 @@
         <v>81</v>
       </c>
       <c r="C58" s="5"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
     </row>
@@ -3897,17 +3778,6 @@
         <v>92</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
       <c r="O59" s="5"/>
       <c r="P59" s="5"/>
     </row>
@@ -3917,21 +3787,12 @@
         <v>96</v>
       </c>
       <c r="C60" s="5"/>
-      <c r="D60" s="14" t="s">
+      <c r="D60" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
       <c r="O60" s="5"/>
       <c r="P60" s="5"/>
     </row>
@@ -3941,21 +3802,12 @@
         <v>97</v>
       </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="14" t="s">
+      <c r="D61" t="s">
         <v>15</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" t="s">
         <v>98</v>
       </c>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
     </row>
@@ -3963,217 +3815,64 @@
       <c r="A62" s="4"/>
       <c r="B62" s="8"/>
       <c r="C62" s="10"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="14"/>
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
-      <c r="B64" s="14" t="s">
+      <c r="B64" t="s">
         <v>93</v>
       </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
       <c r="O65" s="5"/>
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
       <c r="O68" s="5"/>
       <c r="P68" s="5"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
       <c r="O69" s="5"/>
       <c r="P69" s="5"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="N70" s="14"/>
       <c r="O70" s="5"/>
       <c r="P70" s="5"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
       <c r="O71" s="5"/>
       <c r="P71" s="5"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
       <c r="O72" s="5"/>
       <c r="P72" s="5"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
       <c r="O73" s="5"/>
       <c r="P73" s="5"/>
     </row>
@@ -4217,4 +3916,516 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DD83A9-F54B-524A-843D-F9CE52EDEE61}">
+  <dimension ref="A3:O59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="5"/>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="5"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="5"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="5"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="5"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="5"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="8"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 07 - range 02
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D63A04-11DB-2A4A-9F1A-49444CAAA13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726A50A7-60ED-2744-92DA-6CC6FA83A763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="5" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
+    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="6" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
   </bookViews>
   <sheets>
     <sheet name="If Else" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="While" sheetId="4" r:id="rId4"/>
     <sheet name="Break Continue" sheetId="5" r:id="rId5"/>
     <sheet name="Exe 07 - range 01" sheetId="6" r:id="rId6"/>
+    <sheet name="Exe 07 - range 02" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="120">
   <si>
     <t>構成</t>
   </si>
@@ -382,6 +383,24 @@
   </si>
   <si>
     <t>index = 1, 2</t>
+  </si>
+  <si>
+    <t>exe_07_range_02.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_07_range_02.py</t>
+  </si>
+  <si>
+    <t>myList = ['a', 'b']</t>
+  </si>
+  <si>
+    <t>n = 4</t>
+  </si>
+  <si>
+    <t>result = ["{}-{}".format(elm, index) for index in range(1, n+1) for elm in myList ]</t>
+  </si>
+  <si>
+    <t>python3 exe_07_range_02.py</t>
   </si>
 </sst>
 </file>
@@ -1088,6 +1107,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>382408</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8CA0023-5F0A-AB65-62E2-883B74289056}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914400" y="9829800"/>
+          <a:ext cx="12676008" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3922,8 +3990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DD83A9-F54B-524A-843D-F9CE52EDEE61}">
   <dimension ref="A3:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4065,7 +4133,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
-      <c r="D22" s="13" t="s">
+      <c r="D22" t="s">
         <v>85</v>
       </c>
       <c r="F22" s="5"/>
@@ -4156,68 +4224,44 @@
       <c r="B36" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
       <c r="F43" s="5"/>
       <c r="G43" t="s">
         <v>15</v>
@@ -4230,34 +4274,22 @@
       <c r="B44" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -4288,123 +4320,33 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="14" t="s">
+      <c r="B52" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
       <c r="O52" s="5"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
       <c r="O53" s="5"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
       <c r="O54" s="5"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
       <c r="O55" s="5"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
       <c r="O56" s="5"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
       <c r="O57" s="5"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
       <c r="O58" s="5"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -4428,4 +4370,529 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F657561F-876C-F64A-B194-6F92727F6D2F}">
+  <dimension ref="A3:Q56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="10"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="3"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="4"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="4"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="4"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="4"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="5"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="4"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 08 - count
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726A50A7-60ED-2744-92DA-6CC6FA83A763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8381EF05-6CC5-A147-A363-DD7A1094919D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="6" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
+    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="7" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
   </bookViews>
   <sheets>
     <sheet name="If Else" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Break Continue" sheetId="5" r:id="rId5"/>
     <sheet name="Exe 07 - range 01" sheetId="6" r:id="rId6"/>
     <sheet name="Exe 07 - range 02" sheetId="7" r:id="rId7"/>
+    <sheet name="Exe 08 - count" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="136">
   <si>
     <t>構成</t>
   </si>
@@ -401,6 +402,54 @@
   </si>
   <si>
     <t>python3 exe_07_range_02.py</t>
+  </si>
+  <si>
+    <t>exe_08_count.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_08_count.py</t>
+  </si>
+  <si>
+    <t>Từ 1 chuỗi ban đầu thống kê xem các ký tự trong chuỗi đó xuất hiện bao nhiêu lần</t>
+  </si>
+  <si>
+    <t># Input     : google.com</t>
+  </si>
+  <si>
+    <t># Output    : {'g':2, 'o':3, 'l':1, 'e': 1, '.': 1, 'c':1, 'm':1}</t>
+  </si>
+  <si>
+    <t>myString = 'google.com'</t>
+  </si>
+  <si>
+    <t>result   = {}</t>
+  </si>
+  <si>
+    <t>for n in myString:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    keys = result.keys()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if n in keys:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        result[n] += 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        result[n] = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>for elm in result:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print(elm, ": ", result[elm])</t>
+  </si>
+  <si>
+    <t>python3 exe_08_count.py</t>
   </si>
 </sst>
 </file>
@@ -1156,6 +1205,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>301572</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AA3D84A-02FB-1BE5-C748-427975C449C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="11480800"/>
+          <a:ext cx="10867972" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4376,8 +4474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F657561F-876C-F64A-B194-6F92727F6D2F}">
   <dimension ref="A3:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4574,7 +4672,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="13" t="s">
+      <c r="C30" t="s">
         <v>101</v>
       </c>
       <c r="F30" s="5"/>
@@ -4619,73 +4717,38 @@
       <c r="B37" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B38" s="4"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
       <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
       <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -4720,156 +4783,37 @@
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
-      <c r="B48" s="14" t="s">
+      <c r="B48" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
       <c r="Q48" s="5"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
       <c r="Q49" s="5"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
       <c r="Q50" s="5"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
       <c r="Q51" s="5"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
       <c r="Q52" s="5"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
       <c r="Q53" s="5"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
       <c r="Q54" s="5"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
       <c r="Q55" s="5"/>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
@@ -4895,4 +4839,627 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560840D9-9CFE-EE45-A3AB-1F0198E17A35}">
+  <dimension ref="A2:O68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B50" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="10"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="3"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="5"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="14"/>
+      <c r="O57" s="5"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="5"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="5"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="5"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="14"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="5"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="5"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="5"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="5"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="5"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="5"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="5"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A68" s="8"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 09 - longest
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
+++ b/me/1.Lap-trinh-python/1.Lap-trinh-python/3.controll-Statements-if-elseif-while-do-forloop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8381EF05-6CC5-A147-A363-DD7A1094919D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C48FED-18FF-8847-ABC4-C88240A16765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="7" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
+    <workbookView xWindow="1800" yWindow="1280" windowWidth="30140" windowHeight="18360" activeTab="8" xr2:uid="{252E667D-972C-5D4B-9BF9-9F9D23E3C2C1}"/>
   </bookViews>
   <sheets>
     <sheet name="If Else" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Exe 07 - range 01" sheetId="6" r:id="rId6"/>
     <sheet name="Exe 07 - range 02" sheetId="7" r:id="rId7"/>
     <sheet name="Exe 08 - count" sheetId="8" r:id="rId8"/>
+    <sheet name="Exe 09 - longest" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="151">
   <si>
     <t>構成</t>
   </si>
@@ -450,6 +451,51 @@
   </si>
   <si>
     <t>python3 exe_08_count.py</t>
+  </si>
+  <si>
+    <t>exe_09_longest.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_09_longest.py</t>
+  </si>
+  <si>
+    <t># Input     : Cho 1 list chứa các chuỗi</t>
+  </si>
+  <si>
+    <t># Output    : Phần tử có chiều dài lớn nhất</t>
+  </si>
+  <si>
+    <t># Ví dụ     : ["PHP", "Exercises", "Backend"] phần tử có chiều dài lớn nhất: Exercises</t>
+  </si>
+  <si>
+    <t>myList = ["PHP", "Exercises", "Backend"]</t>
+  </si>
+  <si>
+    <t>result  = ""</t>
+  </si>
+  <si>
+    <t>count   = 0</t>
+  </si>
+  <si>
+    <t># for elm in myList:</t>
+  </si>
+  <si>
+    <t>#     if len(elm) &gt; count:</t>
+  </si>
+  <si>
+    <t>#         count = len(elm)</t>
+  </si>
+  <si>
+    <t>#         result= elm</t>
+  </si>
+  <si>
+    <t># print(result)</t>
+  </si>
+  <si>
+    <t>result = max(myList, key = len)</t>
+  </si>
+  <si>
+    <t>python3 exe_09_longest.py</t>
   </si>
 </sst>
 </file>
@@ -1254,6 +1300,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>174918</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B4D322F-019E-554A-4BA6-959DC288CE65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939799" y="12293600"/>
+          <a:ext cx="11617619" cy="1168400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4845,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560840D9-9CFE-EE45-A3AB-1F0198E17A35}">
   <dimension ref="A2:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5055,7 +5150,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="4"/>
-      <c r="C32" s="13" t="s">
+      <c r="C32" t="s">
         <v>114</v>
       </c>
       <c r="F32" s="5"/>
@@ -5098,115 +5193,76 @@
       <c r="B39" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="4"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -5237,208 +5293,53 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
-      <c r="B56" s="14" t="s">
+      <c r="B56" t="s">
         <v>135</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
       <c r="O56" s="5"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
       <c r="O57" s="5"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
       <c r="O58" s="5"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
       <c r="O59" s="5"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
       <c r="O60" s="5"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
       <c r="O61" s="5"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
-      <c r="N62" s="14"/>
       <c r="O62" s="5"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="14"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
       <c r="O63" s="5"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
       <c r="O64" s="5"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
       <c r="O65" s="5"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
       <c r="O66" s="5"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
       <c r="O67" s="5"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
@@ -5462,4 +5363,610 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC1127F-8DA1-CF45-BA10-577B5612A94C}">
+  <dimension ref="A3:P67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="4"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="4"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="10"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="14"/>
+      <c r="P60" s="5"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="14"/>
+      <c r="N61" s="14"/>
+      <c r="O61" s="14"/>
+      <c r="P61" s="5"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="14"/>
+      <c r="P62" s="5"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="4"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="N63" s="14"/>
+      <c r="O63" s="14"/>
+      <c r="P63" s="5"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="5"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A65" s="4"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="5"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A66" s="4"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="14"/>
+      <c r="P66" s="5"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A67" s="8"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="9"/>
+      <c r="P67" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>